<commit_message>
All of degree in HW5 commited
</commit_message>
<xml_diff>
--- a/Degrees.xlsx
+++ b/Degrees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\Tamrin AP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6FDD80-CD22-43CE-9127-6C1B6EA62F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB996E5-4A3A-4239-BE55-7D7CA7E1D2DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>5.2: -2 for bug in menu</t>
+  </si>
+  <si>
+    <t>5.1: not exist overwrite and vircual and program trminate every input, not good output. 5.2: add func don’t work</t>
+  </si>
+  <si>
+    <t>5.2: rule is incorrect but have this message</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1135,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1419,9 +1425,15 @@
         <v>13</v>
       </c>
       <c r="D11" s="45"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="15">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
       <c r="H11" s="30"/>
       <c r="I11" s="36"/>
       <c r="J11" s="39"/>
@@ -1442,9 +1454,15 @@
         <v>14</v>
       </c>
       <c r="D12" s="45"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="15">
+        <v>30</v>
+      </c>
+      <c r="F12" s="16">
+        <v>60</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
+      </c>
       <c r="H12" s="30"/>
       <c r="I12" s="36"/>
       <c r="J12" s="39"/>
@@ -1452,7 +1470,9 @@
       <c r="L12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="56"/>
+      <c r="M12" s="56" t="s">
+        <v>23</v>
+      </c>
       <c r="N12" s="60"/>
       <c r="O12" s="61"/>
     </row>
@@ -1465,14 +1485,22 @@
         <v>15</v>
       </c>
       <c r="D13" s="45"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="E13" s="18">
+        <v>100</v>
+      </c>
+      <c r="F13" s="19">
+        <v>85</v>
+      </c>
+      <c r="G13" s="20">
+        <v>10</v>
+      </c>
       <c r="H13" s="31"/>
       <c r="I13" s="40"/>
       <c r="J13" s="41"/>
       <c r="K13" s="42"/>
-      <c r="M13" s="62"/>
+      <c r="M13" s="62" t="s">
+        <v>24</v>
+      </c>
       <c r="N13" s="63"/>
       <c r="O13" s="64"/>
     </row>

</xml_diff>

<commit_message>
all degree of HW6 commited
</commit_message>
<xml_diff>
--- a/Degrees.xlsx
+++ b/Degrees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\Tamrin AP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13527DD0-46AF-4C31-AA70-A5AD0351E448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363D6D5C-2F0D-404E-9324-2FDD62711A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>توضیحات</t>
   </si>
   <si>
-    <t>5.2: rule is incorrect but have this message</t>
-  </si>
-  <si>
     <t>6: not good menu,MeliID not work,menu in admin option not work good, bug in file data,not search option in admin panel</t>
   </si>
   <si>
@@ -126,7 +123,10 @@
     <t>6:file bug,bug in add and remove product,search and changepass not consist,SID and MeliID false,chance not consist,(total degree just for menu)</t>
   </si>
   <si>
-    <t xml:space="preserve">5.1: not exist overwrite and vircual and program trminate every input, not good output. 5.2: add func don’t work 6:file address bug,menu is so bad, have exception in admin panel,changepass not work,in user panel exception </t>
+    <t>5.1: not exist overwrite and vircual and program trminate every input, not good output. 5.2: add func don’t work 6:file address bug,menu is so bad, have exception in admin panel,changepass not work,in user panel exception (total degree for menu and check email)</t>
+  </si>
+  <si>
+    <t>5.2: rule is incorrect but have this message 6:file address bug,</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="M4" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N4" s="56"/>
       <c r="O4" s="57"/>
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="M5" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N5" s="56"/>
       <c r="O5" s="57"/>
@@ -1324,7 +1324,7 @@
         <v>16</v>
       </c>
       <c r="M6" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" s="56"/>
       <c r="O6" s="57"/>
@@ -1373,13 +1373,13 @@
         <v>100</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="17">
         <v>10</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="36"/>
       <c r="J8" s="39"/>
@@ -1388,7 +1388,7 @@
         <v>16</v>
       </c>
       <c r="M8" s="43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N8" s="44"/>
       <c r="O8" s="45"/>
@@ -1421,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="M9" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N9" s="44"/>
       <c r="O9" s="45"/>
@@ -1454,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="M10" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N10" s="44"/>
       <c r="O10" s="45"/>
@@ -1487,7 +1487,7 @@
         <v>16</v>
       </c>
       <c r="M11" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N11" s="44"/>
       <c r="O11" s="45"/>
@@ -1520,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="M12" s="43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N12" s="44"/>
       <c r="O12" s="45"/>
@@ -1543,12 +1543,14 @@
       <c r="G13" s="20">
         <v>10</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="31">
+        <v>97</v>
+      </c>
       <c r="I13" s="40"/>
       <c r="J13" s="41"/>
       <c r="K13" s="42"/>
       <c r="M13" s="46" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="N13" s="47"/>
       <c r="O13" s="48"/>

</xml_diff>

<commit_message>
all degree of HW7 commited and job done
</commit_message>
<xml_diff>
--- a/Degrees.xlsx
+++ b/Degrees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\Tamrin AP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E0ED47-21A6-4DAA-927B-151BF5CA8CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3025437D-6DE8-4181-A794-323995C4DBEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7800" yWindow="2904" windowWidth="17280" windowHeight="8964" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -96,44 +96,47 @@
     <t>توضیحات</t>
   </si>
   <si>
-    <t>6: not good menu,MeliID not work,menu in admin option not work good, bug in file data,not search option in admin panel</t>
-  </si>
-  <si>
-    <t>6:bug in chance,</t>
-  </si>
-  <si>
     <t>5.3:2 for solve and new 6:bug in select user,MeliID not work</t>
   </si>
   <si>
-    <t>6:expction in chance,chance not work,MeliID not work,</t>
-  </si>
-  <si>
     <t>100 90per(90)</t>
   </si>
   <si>
     <t>82 70Per(57.5)</t>
   </si>
   <si>
-    <t>5.2: -2 for bug in menu 6:customer panel not work, showcustomer not complete</t>
-  </si>
-  <si>
     <t>6:file bug,bug in add and remove product,search and changepass not consist,SID and MeliID false,chance not consist,(total degree just for menu)</t>
   </si>
   <si>
-    <t>5.1: not exist overwrite and vircual and program trminate every input, not good output. 5.2: add func don’t work 6:file address bug,menu is so bad, have exception in admin panel,changepass not work,in user panel exception (total degree for menu and check email)</t>
-  </si>
-  <si>
     <t>6:WPF 7.1:unit test</t>
   </si>
   <si>
     <t>5.2: rule is incorrect but have this message 6:file address bug 7.1:not implict and explict for operator and not line in main method</t>
+  </si>
+  <si>
+    <t>6: not good menu,MeliID not work,menu in admin option not work good, bug in file data,not search option in admin panel 7.3:Q1 repeat,Q3,Q4,Q6</t>
+  </si>
+  <si>
+    <t>6:bug in chance 7.3:Q6</t>
+  </si>
+  <si>
+    <t>7.3=5+5(Code+Anwser)</t>
+  </si>
+  <si>
+    <t>6:expction in chance,chance not work,MeliID not work 7.3:Q10</t>
+  </si>
+  <si>
+    <t>5.1: not exist overwrite and vircual and program trminate every input, not good output. 5.2: add func don’t work 6:file address bug,menu is so bad, have exception in admin panel,changepass not work,in user panel exception (total degree for menu and check email)  7.3:Q10</t>
+  </si>
+  <si>
+    <t>5.2: -2 for bug in menu 6:customer panel not work, showcustomer not complete  7.3:Q6,Q10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +199,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -247,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -649,11 +657,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -838,6 +857,15 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BD848E-E297-4097-8BEE-9ABC561FDC7A}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1169,7 +1197,8 @@
     <col min="13" max="13" width="11.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.88671875" customWidth="1"/>
     <col min="15" max="15" width="24.109375" customWidth="1"/>
-    <col min="16" max="17" width="12.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1256,12 +1285,14 @@
       <c r="J4" s="34">
         <v>100</v>
       </c>
-      <c r="K4" s="35"/>
+      <c r="K4" s="35">
+        <v>82</v>
+      </c>
       <c r="L4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="54" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N4" s="55"/>
       <c r="O4" s="56"/>
@@ -1293,12 +1324,14 @@
       <c r="J5" s="38">
         <v>100</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="37">
+        <v>95</v>
+      </c>
       <c r="L5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="N5" s="55"/>
       <c r="O5" s="56"/>
@@ -1330,12 +1363,14 @@
       <c r="J6" s="38">
         <v>100</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="37">
+        <v>100</v>
+      </c>
       <c r="L6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N6" s="55"/>
       <c r="O6" s="56"/>
@@ -1390,13 +1425,13 @@
         <v>100</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" s="17">
         <v>10</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I8" s="36">
         <v>100</v>
@@ -1404,12 +1439,14 @@
       <c r="J8" s="38">
         <v>100</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="37">
+        <v>90</v>
+      </c>
       <c r="L8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M8" s="42" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N8" s="43"/>
       <c r="O8" s="44"/>
@@ -1441,12 +1478,14 @@
       <c r="J9" s="38">
         <v>100</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="37">
+        <v>100</v>
+      </c>
       <c r="L9" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M9" s="42" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="N9" s="43"/>
       <c r="O9" s="44"/>
@@ -1478,12 +1517,14 @@
       <c r="J10" s="38">
         <v>100</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="37">
+        <v>90</v>
+      </c>
       <c r="L10" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N10" s="43"/>
       <c r="O10" s="44"/>
@@ -1522,7 +1563,7 @@
         <v>16</v>
       </c>
       <c r="M11" s="42" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N11" s="43"/>
       <c r="O11" s="44"/>
@@ -1554,12 +1595,14 @@
       <c r="J12" s="38">
         <v>100</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="37">
+        <v>95</v>
+      </c>
       <c r="L12" s="21" t="s">
         <v>16</v>
       </c>
       <c r="M12" s="42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N12" s="43"/>
       <c r="O12" s="44"/>
@@ -1591,14 +1634,16 @@
       <c r="J13" s="40">
         <v>100</v>
       </c>
-      <c r="K13" s="41"/>
+      <c r="K13" s="41">
+        <v>100</v>
+      </c>
       <c r="M13" s="45" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N13" s="46"/>
       <c r="O13" s="47"/>
     </row>
-    <row r="14" spans="1:15" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -1610,7 +1655,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="22"/>
       <c r="C15" s="25"/>
       <c r="D15" s="22"/>
@@ -1621,8 +1666,13 @@
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M15" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+    </row>
+    <row r="16" spans="1:15" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1707,7 +1757,8 @@
       <c r="K22" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="M15:O15"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>

</xml_diff>